<commit_message>
Write local csv file; remove the date-time str from local db file name so that all data are written into a single db file.
</commit_message>
<xml_diff>
--- a/design_docs/数据库结构.xlsx
+++ b/design_docs/数据库结构.xlsx
@@ -28,218 +28,218 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="73">
   <si>
     <t>库名</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>表1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>experiment</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>表名</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>列名</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>列说明</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>表2</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>type</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>desc</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>实验开始的日期。格式为“YYYY-MM-DD”。字符串。不能为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>描述性文字。字符串。可以为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>datum</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>pos</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>位置。字符串。不能为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>lambda</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>data</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>time</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>描述性文字，对本次实验的说明。字符串。可以为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>光波波长。目前有19个可选值，后续可能增加。数字。不能为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>desc</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>2022-10-14</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>0001</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>敏感型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>额头</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>首次在佰鸿对志愿者进行数据采集，10月14日至21日期间采集了5种类型。使用原始设备进行采集。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>dev_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>表3</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>device</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>expt_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>expt_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>dev_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>addr</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>表4</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>皮肤归属的类型。目前有5个可选值：干燥型，敏感型，痤疮型，皱纹型，色沉型。后续可能增加。字符串。不能为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>object</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>obj_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>obj_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>对象编号。与object表的obj_id关联。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>采集到的数据。数字。不能为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>设备标识。取值建议按数字递增。字符串。
 Primary Key</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>采集对象编号。如果是人，一般一人一个编号；但如果存在一个人属于多种类型的情况，则会有多个编号，每种类型一个。字符串。
 Primary Key</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>设备MAC地址。格式为“HH:HH:HH:HH:HH:HH”。“H”为十六进制字符。字符串。可以为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>描述性文字。对设备进行说明。字符串。可以为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>实验编号。取值建议按数字递增。字符串。
 Primary Key</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>采集日期。格式参考experiment表的date字段。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>采集时间。格式为“HH:MM:SS”，24小时制。字符串。不能为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>27:A5:D2:1E:67:DD</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>原始设备</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>Z0015</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>皱纹型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>2022/10/20</t>
@@ -249,35 +249,35 @@
   </si>
   <si>
     <t>左内眼角</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>采集数据使用的设备标识。与device表的dev_id关联。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>实验编号。与experiment表的expt_id关联。可以为空。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>detector</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>视图1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>datum_view</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>rec_id</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>自动生成的记录id（Auto Increment）。作为Primary Key。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>FROM datum</t>
@@ -290,15 +290,15 @@
   </si>
   <si>
     <t>视图创建方式：</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>CREATE VIEW datum_view AS</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>skin_type</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -314,11 +314,19 @@
       </rPr>
       <t>bject表的skin_type关联。</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dev_addr</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集时间。格式参考experiment表的time字段。</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>SELECT datum.dev_id, datum.obj_id, object.</t>
+      <t>SELECT datum.obj_id, object.</t>
     </r>
     <r>
       <rPr>
@@ -328,34 +336,16 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>skin_</t>
+      <t>skin_type, datum.pos, datum.lambda, datum.data, datum.date,  datum.time, datum.dev_id, datum.expt_id</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>type, datum.pos, datum.lambda, datum.data, datum.date,  datum.time, datum.expt_id</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>dev_addr</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集时间。格式参考experiment表的time字段。</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +353,13 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -570,119 +567,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1101,7 +1098,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>9</v>
@@ -1191,8 +1188,8 @@
       <c r="F21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="38" t="s">
-        <v>72</v>
+      <c r="G21" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="H21" s="24" t="s">
         <v>56</v>
@@ -1222,28 +1219,28 @@
         <v>4</v>
       </c>
       <c r="B25" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="25" t="s">
         <v>27</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>30</v>
@@ -1253,29 +1250,29 @@
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="24" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="J26" s="26" t="s">
         <v>57</v>
@@ -1292,8 +1289,8 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="B29" s="37" t="s">
-        <v>70</v>
+      <c r="B29" s="38" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1312,7 +1309,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2451,7 +2448,7 @@
       <c r="D56" s="23"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
remote db 01: still crash...
</commit_message>
<xml_diff>
--- a/design_docs/数据库结构.xlsx
+++ b/design_docs/数据库结构.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12135" windowHeight="5243"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12135" windowHeight="5243" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="原型" sheetId="1" r:id="rId1"/>
     <sheet name="样例" sheetId="3" r:id="rId2"/>
+    <sheet name="History" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,221 +26,213 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="74">
   <si>
     <t>库名</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>表1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>experiment</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>表名</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>列名</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>列说明</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>表2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>desc</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>实验开始的日期。格式为“YYYY-MM-DD”。字符串。不能为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>描述性文字。字符串。可以为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>datum</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>pos</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>位置。字符串。不能为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>lambda</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>data</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>time</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>描述性文字，对本次实验的说明。字符串。可以为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>光波波长。目前有19个可选值，后续可能增加。数字。不能为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>desc</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2022-10-14</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>0001</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>敏感型</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>额头</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>首次在佰鸿对志愿者进行数据采集，10月14日至21日期间采集了5种类型。使用原始设备进行采集。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>dev_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>表3</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>device</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>expt_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>expt_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>dev_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>addr</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>表4</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>皮肤归属的类型。目前有5个可选值：干燥型，敏感型，痤疮型，皱纹型，色沉型。后续可能增加。字符串。不能为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>object</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>obj_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>obj_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>对象编号。与object表的obj_id关联。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>采集到的数据。数字。不能为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>设备标识。取值建议按数字递增。字符串。
 Primary Key</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>采集对象编号。如果是人，一般一人一个编号；但如果存在一个人属于多种类型的情况，则会有多个编号，每种类型一个。字符串。
 Primary Key</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>设备MAC地址。格式为“HH:HH:HH:HH:HH:HH”。“H”为十六进制字符。字符串。可以为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>描述性文字。对设备进行说明。字符串。可以为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>实验编号。取值建议按数字递增。字符串。
 Primary Key</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>采集日期。格式参考experiment表的date字段。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>采集时间。格式为“HH:MM:SS”，24小时制。字符串。不能为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>27:A5:D2:1E:67:DD</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>原始设备</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Z0015</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>皱纹型</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2022/10/20</t>
@@ -249,35 +242,35 @@
   </si>
   <si>
     <t>左内眼角</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>采集数据使用的设备标识。与device表的dev_id关联。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>实验编号。与experiment表的expt_id关联。可以为空。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>detector</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>视图1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>datum_view</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>rec_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>自动生成的记录id（Auto Increment）。作为Primary Key。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>FROM datum</t>
@@ -290,15 +283,15 @@
   </si>
   <si>
     <t>视图创建方式：</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>CREATE VIEW datum_view AS</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>skin_type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -314,15 +307,15 @@
       </rPr>
       <t>bject表的skin_type关联。</t>
     </r>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>dev_addr</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>采集时间。格式参考experiment表的time字段。</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -338,14 +331,25 @@
       </rPr>
       <t>skin_type, datum.pos, datum.lambda, datum.data, datum.date,  datum.time, datum.dev_id, datum.expt_id</t>
     </r>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>descpt</t>
+  </si>
+  <si>
+    <t>descpt</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>“desc”不能在mysql中是关键字，不能作为列名。更改为“descpt”。</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +357,13 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -563,123 +574,126 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -986,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.4" thickBot="1">
@@ -1007,16 +1021,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75.400000000000006" thickBot="1">
@@ -1024,16 +1038,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.4" thickBot="1">
@@ -1046,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.149999999999999" thickBot="1">
@@ -1054,13 +1068,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="105.4" thickBot="1">
@@ -1068,18 +1082,18 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.4" thickBot="1">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.149999999999999" thickBot="1">
@@ -1087,7 +1101,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.149999999999999" thickBot="1">
@@ -1095,13 +1109,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="90.4" thickBot="1">
@@ -1109,13 +1123,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1126,7 +1140,7 @@
     </row>
     <row r="18" spans="1:10" ht="15.4" thickBot="1">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75">
@@ -1134,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75">
@@ -1142,31 +1156,31 @@
         <v>4</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="G20" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="29" t="s">
-        <v>18</v>
-      </c>
       <c r="H20" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120">
@@ -1174,36 +1188,36 @@
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.4" thickBot="1">
       <c r="A23" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16.149999999999999" thickBot="1">
@@ -1211,7 +1225,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16.149999999999999" thickBot="1">
@@ -1219,31 +1233,31 @@
         <v>4</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105.4" thickBot="1">
@@ -1251,65 +1265,65 @@
         <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="B27" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="B28" s="34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="B29" s="38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="B32" s="35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1320,7 +1334,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1341,10 +1355,10 @@
     </row>
     <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
@@ -1355,60 +1369,60 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75">
       <c r="A6" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75">
       <c r="A7" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1416,55 +1430,55 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75">
       <c r="A15" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75">
       <c r="A16" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="20" customFormat="1">
       <c r="A17" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E17" s="21">
         <v>354</v>
@@ -1473,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H17" s="19">
         <v>0.60578703703703707</v>
@@ -1481,16 +1495,16 @@
     </row>
     <row r="18" spans="1:8" s="20" customFormat="1">
       <c r="A18" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E18" s="21">
         <v>376</v>
@@ -1499,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H18" s="19">
         <v>0.60578703703703707</v>
@@ -1507,16 +1521,16 @@
     </row>
     <row r="19" spans="1:8" s="20" customFormat="1">
       <c r="A19" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E19" s="21">
         <v>405</v>
@@ -1525,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H19" s="19">
         <v>0.60578703703703707</v>
@@ -1533,16 +1547,16 @@
     </row>
     <row r="20" spans="1:8" s="20" customFormat="1">
       <c r="A20" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E20" s="21">
         <v>450</v>
@@ -1551,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H20" s="19">
         <v>0.60578703703703707</v>
@@ -1559,16 +1573,16 @@
     </row>
     <row r="21" spans="1:8" s="20" customFormat="1">
       <c r="A21" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E21" s="21">
         <v>505</v>
@@ -1577,7 +1591,7 @@
         <v>496</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H21" s="19">
         <v>0.60578703703703707</v>
@@ -1585,16 +1599,16 @@
     </row>
     <row r="22" spans="1:8" s="20" customFormat="1">
       <c r="A22" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E22" s="21">
         <v>560</v>
@@ -1603,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H22" s="19">
         <v>0.60578703703703707</v>
@@ -1611,16 +1625,16 @@
     </row>
     <row r="23" spans="1:8" s="20" customFormat="1">
       <c r="A23" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E23" s="21">
         <v>600</v>
@@ -1629,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H23" s="19">
         <v>0.60578703703703707</v>
@@ -1637,16 +1651,16 @@
     </row>
     <row r="24" spans="1:8" s="20" customFormat="1">
       <c r="A24" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E24" s="21">
         <v>645</v>
@@ -1655,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H24" s="19">
         <v>0.60578703703703707</v>
@@ -1663,16 +1677,16 @@
     </row>
     <row r="25" spans="1:8" s="20" customFormat="1">
       <c r="A25" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E25" s="21">
         <v>680</v>
@@ -1681,7 +1695,7 @@
         <v>487</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H25" s="19">
         <v>0.60578703703703707</v>
@@ -1689,16 +1703,16 @@
     </row>
     <row r="26" spans="1:8" s="20" customFormat="1">
       <c r="A26" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2">
         <v>0</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E26" s="21">
         <v>705</v>
@@ -1707,7 +1721,7 @@
         <v>700</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H26" s="19">
         <v>0.60578703703703707</v>
@@ -1715,16 +1729,16 @@
     </row>
     <row r="27" spans="1:8" s="20" customFormat="1">
       <c r="A27" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2">
         <v>0</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E27" s="21">
         <v>800</v>
@@ -1733,7 +1747,7 @@
         <v>3223</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H27" s="19">
         <v>0.60578703703703707</v>
@@ -1741,16 +1755,16 @@
     </row>
     <row r="28" spans="1:8" s="20" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2">
         <v>0</v>
       </c>
       <c r="C28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E28" s="21">
         <v>850</v>
@@ -1759,7 +1773,7 @@
         <v>2049</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H28" s="19">
         <v>0.60578703703703707</v>
@@ -1767,16 +1781,16 @@
     </row>
     <row r="29" spans="1:8" s="20" customFormat="1">
       <c r="A29" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2">
         <v>0</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E29" s="21">
         <v>910</v>
@@ -1785,7 +1799,7 @@
         <v>268</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H29" s="19">
         <v>0.60578703703703707</v>
@@ -1793,16 +1807,16 @@
     </row>
     <row r="30" spans="1:8" s="20" customFormat="1">
       <c r="A30" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2">
         <v>0</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E30" s="21">
         <v>930</v>
@@ -1811,7 +1825,7 @@
         <v>1704</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H30" s="19">
         <v>0.60578703703703707</v>
@@ -1819,16 +1833,16 @@
     </row>
     <row r="31" spans="1:8" s="20" customFormat="1">
       <c r="A31" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2">
         <v>0</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E31" s="21">
         <v>970</v>
@@ -1837,7 +1851,7 @@
         <v>3516</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H31" s="19">
         <v>0.60578703703703707</v>
@@ -1845,16 +1859,16 @@
     </row>
     <row r="32" spans="1:8" s="20" customFormat="1">
       <c r="A32" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E32" s="21">
         <v>1000</v>
@@ -1863,7 +1877,7 @@
         <v>3432</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H32" s="19">
         <v>0.60578703703703707</v>
@@ -1871,16 +1885,16 @@
     </row>
     <row r="33" spans="1:8" s="20" customFormat="1">
       <c r="A33" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E33" s="21">
         <v>1050</v>
@@ -1889,7 +1903,7 @@
         <v>14829</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H33" s="19">
         <v>0.60578703703703707</v>
@@ -1897,16 +1911,16 @@
     </row>
     <row r="34" spans="1:8" s="20" customFormat="1">
       <c r="A34" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E34" s="21">
         <v>1070</v>
@@ -1915,7 +1929,7 @@
         <v>8216</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H34" s="19">
         <v>0.60578703703703707</v>
@@ -1923,16 +1937,16 @@
     </row>
     <row r="35" spans="1:8" s="20" customFormat="1">
       <c r="A35" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E35" s="21">
         <v>1200</v>
@@ -1941,7 +1955,7 @@
         <v>13214</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H35" s="19">
         <v>0.60578703703703707</v>
@@ -1949,16 +1963,16 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E36" s="21">
         <v>354</v>
@@ -1967,24 +1981,24 @@
         <v>0</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="2">
         <v>0</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E37" s="21">
         <v>376</v>
@@ -1993,24 +2007,24 @@
         <v>0</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" s="2">
         <v>0</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E38" s="21">
         <v>405</v>
@@ -2019,24 +2033,24 @@
         <v>0</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B39" s="2">
         <v>0</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E39" s="21">
         <v>450</v>
@@ -2045,24 +2059,24 @@
         <v>0</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="2">
         <v>0</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E40" s="21">
         <v>505</v>
@@ -2071,24 +2085,24 @@
         <v>275</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" s="2">
         <v>0</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41" s="21">
         <v>560</v>
@@ -2097,24 +2111,24 @@
         <v>0</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" s="2">
         <v>0</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E42" s="21">
         <v>600</v>
@@ -2123,24 +2137,24 @@
         <v>0</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2">
         <v>0</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E43" s="21">
         <v>645</v>
@@ -2149,24 +2163,24 @@
         <v>0</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44" s="2">
         <v>0</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E44" s="21">
         <v>680</v>
@@ -2175,24 +2189,24 @@
         <v>162</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2">
         <v>0</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E45" s="21">
         <v>705</v>
@@ -2201,24 +2215,24 @@
         <v>264</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
         <v>0</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E46" s="21">
         <v>800</v>
@@ -2227,24 +2241,24 @@
         <v>2167</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47" s="2">
         <v>0</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E47" s="21">
         <v>850</v>
@@ -2253,24 +2267,24 @@
         <v>1793</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" s="2">
         <v>0</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E48" s="21">
         <v>910</v>
@@ -2279,24 +2293,24 @@
         <v>98</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2">
         <v>0</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E49" s="21">
         <v>930</v>
@@ -2305,24 +2319,24 @@
         <v>1165</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2">
         <v>0</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E50" s="21">
         <v>970</v>
@@ -2331,24 +2345,24 @@
         <v>2772</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="2">
         <v>0</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E51" s="21">
         <v>1000</v>
@@ -2357,24 +2371,24 @@
         <v>2628</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52" s="2">
         <v>0</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E52" s="21">
         <v>1050</v>
@@ -2383,24 +2397,24 @@
         <v>9959</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53" s="2">
         <v>0</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E53" s="21">
         <v>1070</v>
@@ -2409,24 +2423,24 @@
         <v>6125</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B54" s="2">
         <v>0</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E54" s="21">
         <v>1200</v>
@@ -2435,10 +2449,10 @@
         <v>9700</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2448,8 +2462,37 @@
       <c r="D56" s="23"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9"/>
+  <cols>
+    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="39">
+        <v>44911</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>